<commit_message>
correção de asset, multi inimigos implementado
</commit_message>
<xml_diff>
--- a/maps/zero_cor_sim.xlsx
+++ b/maps/zero_cor_sim.xlsx
@@ -466,16 +466,16 @@
   </sheetPr>
   <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y15" activeCellId="0" sqref="Y15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.328125" defaultRowHeight="85.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="1" style="1" width="5.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="1" style="1" width="15.31"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -548,7 +548,7 @@
       <c r="AD1" s="5"/>
       <c r="AE1" s="5"/>
     </row>
-    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -621,7 +621,7 @@
       <c r="AD2" s="5"/>
       <c r="AE2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -694,7 +694,7 @@
       <c r="AD3" s="5"/>
       <c r="AE3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
@@ -767,7 +767,7 @@
       <c r="AD4" s="5"/>
       <c r="AE4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
@@ -840,7 +840,7 @@
       <c r="AD5" s="5"/>
       <c r="AE5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
@@ -913,7 +913,7 @@
       <c r="AD6" s="5"/>
       <c r="AE6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
@@ -986,7 +986,7 @@
       <c r="AD7" s="5"/>
       <c r="AE7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -1059,7 +1059,7 @@
       <c r="AD8" s="5"/>
       <c r="AE8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
@@ -1132,7 +1132,7 @@
       <c r="AD9" s="5"/>
       <c r="AE9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -1205,7 +1205,7 @@
       <c r="AD10" s="5"/>
       <c r="AE10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1278,7 +1278,7 @@
       <c r="AD11" s="5"/>
       <c r="AE11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1351,7 +1351,7 @@
       <c r="AD12" s="5"/>
       <c r="AE12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="AD13" s="5"/>
       <c r="AE13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
@@ -1497,7 +1497,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
         <v>25</v>
       </c>
@@ -1570,7 +1570,7 @@
       <c r="AD15" s="5"/>
       <c r="AE15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
         <v>25</v>
       </c>
@@ -1643,7 +1643,7 @@
       <c r="AD16" s="5"/>
       <c r="AE16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
         <v>25</v>
       </c>
@@ -1716,7 +1716,7 @@
       <c r="AD17" s="5"/>
       <c r="AE17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
@@ -1789,7 +1789,7 @@
       <c r="AD18" s="5"/>
       <c r="AE18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
         <v>25</v>
       </c>
@@ -1862,7 +1862,7 @@
       <c r="AD19" s="5"/>
       <c r="AE19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="s">
         <v>49</v>
       </c>
@@ -1935,7 +1935,7 @@
       <c r="AD20" s="5"/>
       <c r="AE20" s="5"/>
     </row>
-    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1968,7 +1968,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2001,7 +2001,7 @@
       <c r="AD22" s="5"/>
       <c r="AE22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2034,7 +2034,7 @@
       <c r="AD23" s="5"/>
       <c r="AE23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2067,7 +2067,7 @@
       <c r="AD24" s="5"/>
       <c r="AE24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2100,7 +2100,7 @@
       <c r="AD25" s="5"/>
       <c r="AE25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2133,7 +2133,7 @@
       <c r="AD26" s="5"/>
       <c r="AE26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2166,7 +2166,7 @@
       <c r="AD27" s="5"/>
       <c r="AE27" s="5"/>
     </row>
-    <row r="28" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>

</xml_diff>

<commit_message>
implementado alguns assets de mapa, uma breve otimização ao carregar o mapa refatoração do hud e dos inimigos, array de horda para o teaser
</commit_message>
<xml_diff>
--- a/maps/zero_cor_sim.xlsx
+++ b/maps/zero_cor_sim.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="53">
   <si>
     <t xml:space="preserve">estrutura_central_15</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t xml:space="preserve">chao5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cama_ch5_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cama_ch5_2</t>
   </si>
   <si>
     <t xml:space="preserve">void</t>
@@ -221,7 +227,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,6 +306,12 @@
         <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
@@ -335,7 +347,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -393,6 +405,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -479,8 +495,8 @@
   </sheetPr>
   <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.328125" defaultRowHeight="85.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1672,8 +1688,8 @@
       <c r="E17" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>49</v>
+      <c r="F17" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>8</v>
@@ -1690,8 +1706,8 @@
       <c r="K17" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="L17" s="14" t="s">
-        <v>49</v>
+      <c r="L17" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>8</v>
@@ -1745,8 +1761,8 @@
       <c r="E18" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="14" t="s">
-        <v>49</v>
+      <c r="F18" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>8</v>
@@ -1763,8 +1779,8 @@
       <c r="K18" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="L18" s="14" t="s">
-        <v>49</v>
+      <c r="L18" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>8</v>
@@ -1876,65 +1892,65 @@
       <c r="AE19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="L20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="M20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="N20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="O20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="P20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="R20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="S20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="T20" s="15" t="s">
-        <v>50</v>
+      <c r="A20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="O20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="P20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="R20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="S20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="T20" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="U20" s="5"/>
       <c r="V20" s="5"/>

</xml_diff>